<commit_message>
Removed dependency on RODBC Using readxl instead
</commit_message>
<xml_diff>
--- a/inst/extdata/contrasts.xlsx
+++ b/inst/extdata/contrasts.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dieter\Documents\RPackages\Dmisc2\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="4320" yWindow="165" windowWidth="23655" windowHeight="14310"/>
   </bookViews>
   <sheets>
-    <sheet name="Contrasts" sheetId="1" r:id="rId1"/>
+    <sheet name="peripostinterval" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="aucContr">Contrasts!#REF!</definedName>
-    <definedName name="aucDiffContr">Contrasts!#REF!</definedName>
-    <definedName name="periGroup">Contrasts!#REF!</definedName>
-    <definedName name="perigroupdiff">Contrasts!#REF!</definedName>
-    <definedName name="peripostinterval">Contrasts!$A$1:$I$7</definedName>
+    <definedName name="aucContr">peripostinterval!#REF!</definedName>
+    <definedName name="aucDiffContr">peripostinterval!#REF!</definedName>
+    <definedName name="periGroup">peripostinterval!#REF!</definedName>
+    <definedName name="perigroupdiff">peripostinterval!#REF!</definedName>
+    <definedName name="peripostinterval">peripostinterval!$A$1:$I$7</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -92,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +158,21 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,9 +210,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,9 +244,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,9 +279,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -440,14 +455,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="IX1" sqref="IX1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
@@ -457,7 +472,7 @@
     <col min="258" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:257" ht="86.25">
+    <row r="1" spans="1:257" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -486,7 +501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:257">
+    <row r="2" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -518,7 +533,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:257">
+    <row r="3" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -550,7 +565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:257">
+    <row r="4" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -582,7 +597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:257">
+    <row r="5" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -614,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:257">
+    <row r="6" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -646,7 +661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:257">
+    <row r="7" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -678,9 +693,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:257"/>
-    <row r="9" spans="1:257" hidden="1"/>
-    <row r="10" spans="1:257" hidden="1">
+    <row r="8" spans="1:257" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:257" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:257" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Corrected comment column in sample excel sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/contrasts.xlsx
+++ b/inst/extdata/contrasts.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Put a 1 everywhere</t>
+  </si>
+  <si>
+    <t>Column without period is not used</t>
   </si>
 </sst>
 </file>
@@ -139,10 +142,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,21 +464,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="IX1" sqref="IX1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="256" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="256" width="11.42578125" customWidth="1"/>
     <col min="257" max="257" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="258" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:257" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -500,8 +506,11 @@
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:257" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -529,11 +538,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="IW2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:257" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,11 +570,11 @@
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="IW3" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:257" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -593,11 +602,11 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="IW4" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:257" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -625,11 +634,11 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="IW5" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:257" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -657,11 +666,11 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="IW6" t="s">
+      <c r="J6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:257" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -689,13 +698,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="IW7" t="s">
+      <c r="J7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:257" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:257" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:257" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -707,5 +714,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>